<commit_message>
bugfix & update model files
</commit_message>
<xml_diff>
--- a/ExperimentalData.xlsx
+++ b/ExperimentalData.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/ShallowInterrupt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC21AF66-6B6F-F848-BF90-70B8341CE297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEECF66-EE49-6E4D-9515-0B82BB356581}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="1580" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
+    <workbookView xWindow="8600" yWindow="1580" windowWidth="28040" windowHeight="17440" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
   </bookViews>
   <sheets>
     <sheet name="ShallowVerification" sheetId="1" r:id="rId1"/>
     <sheet name="SpaceEx" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -141,6 +140,15 @@
   </si>
   <si>
     <t>medical-monitor-1</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>UNSATISFIABLE</t>
+  </si>
+  <si>
+    <t>SATISFIABLE</t>
   </si>
 </sst>
 </file>
@@ -498,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FACF2A-E248-534C-8FDA-43D644C552B5}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,9 +521,10 @@
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +549,11 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -552,22 +564,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5914</v>
+        <v>2176</v>
       </c>
       <c r="F2">
-        <v>0.193</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G2">
-        <v>0.313</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,22 +593,25 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5988</v>
+        <v>2214</v>
       </c>
       <c r="F3">
-        <v>0.214</v>
+        <v>2.4E-2</v>
       </c>
       <c r="G3">
-        <v>0.155</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -604,22 +622,25 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>30337</v>
+        <v>11173</v>
       </c>
       <c r="F4">
-        <v>0.42</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G4">
-        <v>2.1829999999999998</v>
+        <v>0.112</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -630,22 +651,25 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>31153</v>
+        <v>11593</v>
       </c>
       <c r="F5">
-        <v>0.45600000000000002</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="G5">
-        <v>2.0539999999999998</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -656,22 +680,25 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>4553</v>
+        <v>1737</v>
       </c>
       <c r="F6">
-        <v>0.19</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="G6">
-        <v>0.17</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -682,22 +709,25 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>4532</v>
+        <v>1730</v>
       </c>
       <c r="F7">
-        <v>0.16</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G7">
-        <v>0.8</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -708,22 +738,25 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>5031</v>
+        <v>1980</v>
       </c>
       <c r="F8">
-        <v>0.16700000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="G8">
-        <v>2.1999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -734,22 +767,25 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>5031</v>
+        <v>1980</v>
       </c>
       <c r="F9">
-        <v>0.16700000000000001</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="G9">
-        <v>2.1999999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -760,22 +796,25 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>7015</v>
+        <v>2695</v>
       </c>
       <c r="F10">
-        <v>0.224</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G10">
-        <v>0.316</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -786,22 +825,25 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>7015</v>
+        <v>2695</v>
       </c>
       <c r="F11">
-        <v>0.251</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G11">
-        <v>0.32300000000000001</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -812,22 +854,25 @@
         <v>12</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>3671</v>
+        <v>1355</v>
       </c>
       <c r="F12">
-        <v>0.222</v>
+        <v>1.4E-2</v>
       </c>
       <c r="G12">
-        <v>0.17</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -838,99 +883,312 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>3671</v>
+        <v>1355</v>
       </c>
       <c r="F13">
-        <v>0.2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G13">
-        <v>6.8000000000000005E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>526</v>
+      </c>
+      <c r="F14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="G14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>519</v>
+      </c>
+      <c r="F15">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1250</v>
+      </c>
+      <c r="F16">
+        <v>1.9E-2</v>
+      </c>
+      <c r="G16">
+        <v>1.6E-2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1235</v>
+      </c>
+      <c r="F17">
+        <v>0.02</v>
+      </c>
+      <c r="G17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1796</v>
+      </c>
+      <c r="F18">
+        <v>0.02</v>
+      </c>
+      <c r="G18">
+        <v>0.01</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1796</v>
+      </c>
+      <c r="F19">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>9418</v>
+      </c>
+      <c r="F20">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G20">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>9485</v>
+      </c>
+      <c r="F21">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G21">
+        <v>0.125</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2350</v>
+      </c>
+      <c r="F22">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G22">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1403</v>
+      </c>
+      <c r="F23">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G23">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -944,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B27D369-23E2-7742-AB4D-D3DD99B416FF}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1400,6 +1658,24 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
+      <c r="D20">
+        <v>7.77</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>667</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1410,6 +1686,24 @@
       </c>
       <c r="C21" t="s">
         <v>0</v>
+      </c>
+      <c r="D21">
+        <v>8.24</v>
+      </c>
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
data: add SpaceEx cases
</commit_message>
<xml_diff>
--- a/ExperimentalData.xlsx
+++ b/ExperimentalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/ShallowInterrupt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCE3BAD-20D9-5A43-8425-3051EAAC053E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2878EB5-9F5A-9C4B-BA6D-F7AFE35F94EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
   </bookViews>
   <sheets>
     <sheet name="SHANNON" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FACF2A-E248-534C-8FDA-43D644C552B5}">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="K105" sqref="K105"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:XFD119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3755,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B27D369-23E2-7742-AB4D-D3DD99B416FF}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3827,6 +3827,9 @@
       <c r="H2">
         <v>3</v>
       </c>
+      <c r="J2">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -3839,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.2030000000000001</v>
+        <v>1.52</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -3853,6 +3856,9 @@
       <c r="H3">
         <v>3</v>
       </c>
+      <c r="J3">
+        <v>195</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -3865,7 +3871,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>0.81200000000000006</v>
+        <v>18.39</v>
       </c>
       <c r="E4">
         <v>27</v>
@@ -3878,6 +3884,9 @@
       </c>
       <c r="H4">
         <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1138</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -3891,7 +3900,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2.4049999999999998</v>
+        <v>64.989999999999995</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -3904,6 +3913,9 @@
       </c>
       <c r="H5">
         <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3324</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -3917,7 +3929,7 @@
         <v>12</v>
       </c>
       <c r="D6">
-        <v>0.158</v>
+        <v>0.39</v>
       </c>
       <c r="E6">
         <v>14</v>
@@ -3930,6 +3942,9 @@
       </c>
       <c r="H6">
         <v>4</v>
+      </c>
+      <c r="J6">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -3943,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.14799999999999999</v>
+        <v>0.53</v>
       </c>
       <c r="E7">
         <v>14</v>
@@ -3956,6 +3971,9 @@
       </c>
       <c r="H7">
         <v>4</v>
+      </c>
+      <c r="J7">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3969,7 +3987,7 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>3600</v>
+        <v>0.59</v>
       </c>
       <c r="E8">
         <v>17</v>
@@ -3982,6 +4000,9 @@
       </c>
       <c r="H8">
         <v>4</v>
+      </c>
+      <c r="J8">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -4009,6 +4030,9 @@
       <c r="H9">
         <v>4</v>
       </c>
+      <c r="J9">
+        <v>45029</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -4035,6 +4059,9 @@
       <c r="H10">
         <v>3</v>
       </c>
+      <c r="J10">
+        <v>442841</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -4078,8 +4105,17 @@
       <c r="D12">
         <v>3600</v>
       </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
       <c r="G12">
         <v>0</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
       </c>
       <c r="J12">
         <v>26898</v>
@@ -4098,8 +4134,17 @@
       <c r="D13">
         <v>3600</v>
       </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
       <c r="G13">
         <v>0</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
       </c>
       <c r="J13">
         <v>59074</v>
@@ -4116,13 +4161,22 @@
         <v>12</v>
       </c>
       <c r="D14">
-        <v>0.114</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
       <c r="J14">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -4136,10 +4190,19 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.13200000000000001</v>
+        <v>0.33</v>
+      </c>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
       </c>
       <c r="G15">
         <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
       </c>
       <c r="J15">
         <v>33</v>
@@ -4156,10 +4219,19 @@
         <v>12</v>
       </c>
       <c r="D16">
-        <v>9.0999999999999998E-2</v>
+        <v>0.24</v>
+      </c>
+      <c r="E16">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
       </c>
       <c r="G16">
         <v>0</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
       </c>
       <c r="J16">
         <v>7</v>
@@ -4176,10 +4248,19 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>8.6999999999999994E-2</v>
+        <v>0.35</v>
+      </c>
+      <c r="E17">
+        <v>26</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
       </c>
       <c r="G17">
         <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
       </c>
       <c r="J17">
         <v>7</v>
@@ -4196,10 +4277,19 @@
         <v>12</v>
       </c>
       <c r="D18">
-        <v>7.0999999999999994E-2</v>
+        <v>0.24</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
       </c>
       <c r="J18">
         <v>8</v>
@@ -4216,10 +4306,19 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.152</v>
+        <v>0.39</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
       </c>
       <c r="J19">
         <v>8</v>
@@ -4265,7 +4364,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>8.24</v>
+        <v>8.91</v>
       </c>
       <c r="E21">
         <v>38</v>
@@ -4293,8 +4392,23 @@
       <c r="C22" t="s">
         <v>12</v>
       </c>
+      <c r="D22">
+        <v>3600</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
       <c r="G22">
         <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>53794</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -4307,8 +4421,23 @@
       <c r="C23" t="s">
         <v>0</v>
       </c>
+      <c r="D23">
+        <v>3600</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
       <c r="G23">
         <v>1</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>53502</v>
       </c>
     </row>
   </sheetData>
@@ -4320,12 +4449,661 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C805B7-70ED-334B-9B50-24490EB235D3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1.2030000000000001</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="E4">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>0.158</v>
+      </c>
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>3600</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3600</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>3600</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>442841</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3600</v>
+      </c>
+      <c r="E11">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>444613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>3600</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>26898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>3600</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>59074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.33</v>
+      </c>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.24</v>
+      </c>
+      <c r="E16">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.35</v>
+      </c>
+      <c r="E17">
+        <v>26</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>0.24</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.39</v>
+      </c>
+      <c r="E19">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>7.77</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>8.91</v>
+      </c>
+      <c r="E21">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>3600</v>
+      </c>
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>53794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>3600</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>53502</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data: update experimental data
</commit_message>
<xml_diff>
--- a/ExperimentalData.xlsx
+++ b/ExperimentalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/ShallowInterrupt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CF65F1-337D-E545-984F-1BCAF3D6A2BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0662F9EA-A62E-7C40-B008-2FA0A8E54D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4171E658-EED0-5747-AC62-02656070F28E}"/>
   </bookViews>
   <sheets>
     <sheet name="SHANNON" sheetId="1" r:id="rId1"/>
@@ -62,48 +62,15 @@
     <t>Feasible</t>
   </si>
   <si>
-    <t>altitude-display-1</t>
-  </si>
-  <si>
-    <t>altitude-display-int-1</t>
-  </si>
-  <si>
-    <t>ADC-bug-int-1</t>
-  </si>
-  <si>
     <t>Int_Num</t>
   </si>
   <si>
     <t>Auto_Num</t>
   </si>
   <si>
-    <t>ADC-bug-d-int-1</t>
-  </si>
-  <si>
     <t>Iteration</t>
   </si>
   <si>
-    <t>car-controller-1</t>
-  </si>
-  <si>
-    <t>csma-aut-1</t>
-  </si>
-  <si>
-    <t>fisher-aut-1</t>
-  </si>
-  <si>
-    <t>hddi-1</t>
-  </si>
-  <si>
-    <t>water-tank-1</t>
-  </si>
-  <si>
-    <t>learning-factory-1</t>
-  </si>
-  <si>
-    <t>medical-monitor-1</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -132,6 +99,39 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>altitude-display</t>
+  </si>
+  <si>
+    <t>altitude-display-int</t>
+  </si>
+  <si>
+    <t>ADC-bug-int</t>
+  </si>
+  <si>
+    <t>ADC-bug-d-int</t>
+  </si>
+  <si>
+    <t>car-controller</t>
+  </si>
+  <si>
+    <t>csma-aut</t>
+  </si>
+  <si>
+    <t>fisher-aut</t>
+  </si>
+  <si>
+    <t>hddi</t>
+  </si>
+  <si>
+    <t>water-tank</t>
+  </si>
+  <si>
+    <t>learning-factory</t>
+  </si>
+  <si>
+    <t>medical-monitor</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18FACF2A-E248-534C-8FDA-43D644C552B5}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:A64"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,7 +533,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -562,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -599,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -628,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -649,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -678,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -744,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -794,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -802,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -918,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -947,7 +947,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
@@ -968,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1005,7 +1005,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -1026,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1034,7 +1034,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -1055,7 +1055,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1063,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1092,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1121,7 +1121,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1208,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1237,7 +1237,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1266,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1295,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1324,7 +1324,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C33" t="s">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1382,7 +1382,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
@@ -1403,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1411,7 +1411,7 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1440,7 +1440,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C37" t="s">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -1469,7 +1469,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1527,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1556,7 +1556,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -1585,7 +1585,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
@@ -1606,7 +1606,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1614,7 +1614,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
@@ -1635,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1643,7 +1643,7 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1672,7 +1672,7 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
         <v>0</v>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1701,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1730,7 +1730,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
@@ -1751,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -1759,7 +1759,7 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
@@ -1780,7 +1780,7 @@
         <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -1788,7 +1788,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -1817,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
         <v>0</v>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -1846,7 +1846,7 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -1875,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
@@ -1896,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -1904,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
         <v>0</v>
@@ -1925,7 +1925,7 @@
         <v>2</v>
       </c>
       <c r="I57" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -1933,7 +1933,7 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
@@ -1954,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -1991,7 +1991,7 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -2020,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C61" t="s">
         <v>0</v>
@@ -2041,7 +2041,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -2049,7 +2049,7 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -2078,7 +2078,7 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C63" t="s">
         <v>0</v>
@@ -2099,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="I63" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2107,7 +2107,7 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
@@ -2128,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2177,19 +2177,19 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2232,7 +2232,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -2267,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2302,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2337,7 +2337,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -2372,7 +2372,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -2407,7 +2407,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -2442,7 +2442,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -2512,7 +2512,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2547,7 +2547,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -2588,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C805B7-70ED-334B-9B50-24490EB235D3}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2616,7 +2616,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -2641,19 +2641,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2661,7 +2661,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -2678,7 +2678,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -2695,19 +2695,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2715,7 +2715,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -2732,7 +2732,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -2749,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -2766,7 +2766,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -2783,7 +2783,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2800,7 +2800,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>

</xml_diff>